<commit_message>
Updated audio asset XL sheet
</commit_message>
<xml_diff>
--- a/DesignDocumentation/AudioAssetFile.xlsx
+++ b/DesignDocumentation/AudioAssetFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifth\OneDrive\Desktop\GAM200 real\DesignDocumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahes\Desktop\Vyv_Lantern\DesignDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14710860-97D8-4AD7-9F78-7E3F227AE630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD26A4FF-5648-4675-B343-93F426596C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{320EB32C-9F1D-4C4B-8606-D6591F7E05AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{320EB32C-9F1D-4C4B-8606-D6591F7E05AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>ASSET NAME</t>
   </si>
@@ -50,18 +50,12 @@
     <t>PRIORITY OF IMPLEMENTATION</t>
   </si>
   <si>
-    <t>BGM.ogg</t>
-  </si>
-  <si>
     <t>DigiPen Sound Library</t>
   </si>
   <si>
     <t>Moderate</t>
   </si>
   <si>
-    <t>Exterior.wav</t>
-  </si>
-  <si>
     <t>Forest.ogg</t>
   </si>
   <si>
@@ -74,54 +68,27 @@
     <t>Descriptions</t>
   </si>
   <si>
-    <t>FM01-9thSense-Loop-1Minute-Sazonoff</t>
-  </si>
-  <si>
-    <t>Background music that is used to accompany each level</t>
-  </si>
-  <si>
-    <t>Jungles_-Background_-Inside-Tunnel_-Leaks-Drip-Snaps_-Birds-Calls-Distant_-Reverby_-Exterior_1</t>
-  </si>
-  <si>
     <t>Primary ambient sound effect used for each level</t>
   </si>
   <si>
     <t>Nature-Forest-Early-Morning</t>
   </si>
   <si>
-    <t>Ambient sound effect used for later levels</t>
-  </si>
-  <si>
     <t>WaterLiquid-Drips_Splats_Gl</t>
   </si>
   <si>
-    <t>Ambient sound effect that will be used when a player enters a level with a water body</t>
-  </si>
-  <si>
     <t>CreaksSqueaks-PulleySqueak_3</t>
   </si>
   <si>
-    <t>Can be used for activating lever or other mechanical objects</t>
-  </si>
-  <si>
     <t>CreaksSqueaks-PulleySquea_3_full</t>
   </si>
   <si>
-    <t>Used when player moves the track mirrors or the freestanding mirrors</t>
-  </si>
-  <si>
     <t xml:space="preserve">LICENSE </t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Interact Sound Effect (Planned)</t>
-  </si>
-  <si>
-    <t>Laser Sound Effect (Planned)</t>
-  </si>
-  <si>
     <t>Plays whenever player interacts with any object with an available prompt</t>
   </si>
   <si>
@@ -140,16 +107,70 @@
     <t>Playes whenever a laser is split into multiple individual lasers</t>
   </si>
   <si>
+    <t xml:space="preserve">Teleporting Sound Effect (Planned) </t>
+  </si>
+  <si>
     <t>Used for when the teleporting mirror is interacted with, plays when mirror changes locations</t>
   </si>
   <si>
-    <t>SCIENCE-FICTION-LASER-GUN-BEAM-BLASTER-SHOT-01</t>
-  </si>
-  <si>
-    <t>Plays when near lasers</t>
-  </si>
-  <si>
-    <t>Teleport.ogg</t>
+    <t>Plays when lasers are shot out of laser emmiters, Electromagnetic sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laser Sound Effect </t>
+  </si>
+  <si>
+    <t>LaserSFX.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interact Sound Effect </t>
+  </si>
+  <si>
+    <t>CheckpointSFX.wav</t>
+  </si>
+  <si>
+    <t>InteractSFX.wav</t>
+  </si>
+  <si>
+    <t>Soundly</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Background music that is used to accompany the game</t>
+  </si>
+  <si>
+    <t>PrimaryAmbience.wav</t>
+  </si>
+  <si>
+    <t>Level Ambience</t>
+  </si>
+  <si>
+    <t>Background music</t>
+  </si>
+  <si>
+    <t>LevelAmbienceSFX.wav</t>
+  </si>
+  <si>
+    <t>UI menu sound effects</t>
+  </si>
+  <si>
+    <t>Plays whenever player clicks a button in the main menu or pause menu</t>
+  </si>
+  <si>
+    <t>UIMenuSFX.wav</t>
+  </si>
+  <si>
+    <t>Ambient sound effect used for later levels (Planned)</t>
+  </si>
+  <si>
+    <t>Ambient sound effect that will be used when a player enters a level with a water body (Planned)</t>
+  </si>
+  <si>
+    <t>Can be used for activating lever or other mechanical objects (Planned)</t>
+  </si>
+  <si>
+    <t>Used when player moves the track mirrors or the freestanding mirrors (Planned)</t>
   </si>
 </sst>
 </file>
@@ -205,9 +226,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +266,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +372,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,28 +522,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471CC0E3-1BF0-4163-92BC-8887D7CB8008}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.41796875" customWidth="1"/>
-    <col min="2" max="2" width="64.20703125" customWidth="1"/>
-    <col min="3" max="3" width="41.83984375" customWidth="1"/>
-    <col min="4" max="4" width="26.41796875" customWidth="1"/>
-    <col min="5" max="5" width="26.5234375" customWidth="1"/>
-    <col min="6" max="6" width="17.7890625" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -534,227 +555,247 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>25</v>
+      <c r="F13" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Audio asset sheet
</commit_message>
<xml_diff>
--- a/DesignDocumentation/AudioAssetFile.xlsx
+++ b/DesignDocumentation/AudioAssetFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahes\Desktop\Vyv_Lantern\DesignDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD26A4FF-5648-4675-B343-93F426596C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AACB02-AC65-4359-8B5F-07F1E35C8EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{320EB32C-9F1D-4C4B-8606-D6591F7E05AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>ASSET NAME</t>
   </si>
@@ -171,6 +171,51 @@
   </si>
   <si>
     <t>Used when player moves the track mirrors or the freestanding mirrors (Planned)</t>
+  </si>
+  <si>
+    <t>UI open and close</t>
+  </si>
+  <si>
+    <t>Plays whenever the player opens or closes the pause menu</t>
+  </si>
+  <si>
+    <t>UIMenuOpen&amp;Close.wav</t>
+  </si>
+  <si>
+    <t>UI open and close (2)</t>
+  </si>
+  <si>
+    <t>Another SFX for UI open and close</t>
+  </si>
+  <si>
+    <t>UIMenuOpenorClose.wav</t>
+  </si>
+  <si>
+    <t>Victory sound</t>
+  </si>
+  <si>
+    <t>Plays a victory sound bite whenever the player completes the game</t>
+  </si>
+  <si>
+    <t>VictorySFX1-4.wav</t>
+  </si>
+  <si>
+    <t>Opening and closing doors</t>
+  </si>
+  <si>
+    <t>Plays a sound for when the player opens a door to a new section</t>
+  </si>
+  <si>
+    <t>DoorOpen&amp;Close.wav</t>
+  </si>
+  <si>
+    <t>Opening and closing doors (2)</t>
+  </si>
+  <si>
+    <t>Another SFX for Opening and closing doors</t>
+  </si>
+  <si>
+    <t>Door(Short).wav</t>
   </si>
 </sst>
 </file>
@@ -522,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471CC0E3-1BF0-4163-92BC-8887D7CB8008}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,6 +843,106 @@
         <v>16</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Priority and source updated on sound asset file
</commit_message>
<xml_diff>
--- a/DesignDocumentation/AudioAssetFile.xlsx
+++ b/DesignDocumentation/AudioAssetFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\OneDrive\Documents\GitHub\Vyv_Lantern\DesignDocumentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahes\Desktop\Vyv_Lantern\DesignDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1550E39F-2C2A-4ACE-A6FA-C04D0A71CD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8967A857-926D-420A-AB9A-9A8266EE0365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{320EB32C-9F1D-4C4B-8606-D6591F7E05AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{320EB32C-9F1D-4C4B-8606-D6591F7E05AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="53">
   <si>
     <t>ASSET NAME</t>
   </si>
@@ -180,6 +180,21 @@
   </si>
   <si>
     <t>VictorySFX2.mp3</t>
+  </si>
+  <si>
+    <t>DigiPen Sound Library</t>
+  </si>
+  <si>
+    <t>Soundly</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
   </si>
 </sst>
 </file>
@@ -546,20 +561,20 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.90625" customWidth="1"/>
-    <col min="2" max="2" width="64.1796875" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="64.21875" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -579,7 +594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -589,11 +604,17 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -603,11 +624,17 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -617,11 +644,17 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -631,11 +664,17 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -645,11 +684,17 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -659,11 +704,17 @@
       <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -673,11 +724,17 @@
       <c r="C8" t="s">
         <v>27</v>
       </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
       <c r="F8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -687,11 +744,17 @@
       <c r="C9" t="s">
         <v>30</v>
       </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>52</v>
+      </c>
       <c r="F9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -701,11 +764,17 @@
       <c r="C10" t="s">
         <v>32</v>
       </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
       <c r="F10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -715,11 +784,17 @@
       <c r="C11" t="s">
         <v>33</v>
       </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
       <c r="F11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -729,11 +804,17 @@
       <c r="C12" t="s">
         <v>34</v>
       </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
       <c r="F12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -743,11 +824,17 @@
       <c r="C13" t="s">
         <v>35</v>
       </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
       <c r="F13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -757,11 +844,17 @@
       <c r="C14" t="s">
         <v>36</v>
       </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
       <c r="F14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -771,11 +864,17 @@
       <c r="C15" t="s">
         <v>44</v>
       </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
       <c r="F15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -784,6 +883,12 @@
       </c>
       <c r="C16" t="s">
         <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>

</xml_diff>